<commit_message>
added delete on all grids
</commit_message>
<xml_diff>
--- a/InventoryManagementForms/bin/Debug/net6.0-windows/Inventory.xlsx
+++ b/InventoryManagementForms/bin/Debug/net6.0-windows/Inventory.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Inventory Item ID</t>
   </si>
@@ -44,13 +44,10 @@
     <t>Supplier Name</t>
   </si>
   <si>
-    <t>20/03/2023</t>
-  </si>
-  <si>
-    <t>21/03/2023</t>
-  </si>
-  <si>
-    <t>24/03/2023</t>
+    <t>25/03/2023</t>
+  </si>
+  <si>
+    <t>01/01/0001</t>
   </si>
 </sst>
 </file>
@@ -136,19 +133,19 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="0">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2" s="0">
         <v>1</v>
       </c>
       <c r="E2" s="0">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>10</v>
@@ -159,19 +156,19 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="0">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C3" s="0">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3" s="0">
         <v>1</v>
       </c>
       <c r="E3" s="0">
-        <v>40</v>
+        <v>899</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>10</v>
@@ -182,7 +179,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="0">
         <v>1</v>
@@ -194,18 +191,18 @@
         <v>1</v>
       </c>
       <c r="E4" s="0">
-        <v>899</v>
+        <v>8000</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="0">
         <v>1</v>
@@ -217,21 +214,21 @@
         <v>1</v>
       </c>
       <c r="E5" s="0">
-        <v>8000</v>
+        <v>51</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B6" s="0">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C6" s="0">
         <v>1</v>
@@ -240,36 +237,36 @@
         <v>1</v>
       </c>
       <c r="E6" s="0">
-        <v>51</v>
+        <v>1</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B7" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C7" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" s="0">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E7" s="0">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>